<commit_message>
Playing with Ultrasonic sensor
</commit_message>
<xml_diff>
--- a/First-Sprint.xlsx
+++ b/First-Sprint.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Easy Driving Mode</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Youssef Osama</t>
+  </si>
+  <si>
+    <t>Mohamed Aladdin</t>
+  </si>
+  <si>
+    <t>Youssef Moro</t>
   </si>
 </sst>
 </file>
@@ -213,20 +219,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -513,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,35 +529,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="5" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="9"/>
@@ -564,10 +570,10 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -579,17 +585,19 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E6" s="9"/>
@@ -598,6 +606,9 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
+      <c r="K6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E7" s="9"/>
@@ -606,7 +617,9 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E8" s="9"/>
@@ -617,12 +630,12 @@
       <c r="J8" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
       <c r="E11" s="9" t="s">
         <v>3</v>
       </c>
@@ -636,10 +649,10 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -651,17 +664,19 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E14" s="9"/>
@@ -681,93 +696,93 @@
       <c r="K15" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="8" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
       <c r="K18" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
       <c r="K19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
     </row>
     <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>

</xml_diff>